<commit_message>
update article generator, bump prompts xlsx
</commit_message>
<xml_diff>
--- a/resources/prompts.xlsx
+++ b/resources/prompts.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Documents\work\IEF\ai-podcast\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B19D10D-99F8-4F97-822A-CDB6F091299E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACA19A9-2375-4F7F-BEDA-150CBC66B7BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24045" windowHeight="13005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,181 +25,116 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+  <si>
+    <t>Maintain a neutral tone and provide clear, helpful, and detailed responses.</t>
+  </si>
+  <si>
+    <t>Provide thorough, neutral answers. Include references from official, governmental, or otherwise credible sources, and ensure the URLs are as authoritative as possible.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Provide a neutral, well-structured outline for a Wikipedia-style article.</t>
+  </si>
+  <si>
+    <t>You are an expert article writer specialized in creating Wikipedia-style content. Maintain a neutral tone and follow standard Wikipedia guidelines for structure and references.</t>
+  </si>
+  <si>
+    <t>gpt</t>
+  </si>
+  <si>
+    <t>perplexity</t>
+  </si>
   <si>
     <t>Prompt</t>
   </si>
   <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>projects</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
     <t>System prompt</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>index</t>
-  </si>
-  <si>
-    <t>model</t>
+    <t>We have 5 questions about "${topic}". Please answer each question thoroughly, focusing on official, governmental, or highly credible sources. For each question:\n\n1) Provide a concise yet informative answer.\n2) List authoritative references/URLs where more information can be found.\n\nQuestions:\n1. ${question_1}\n2. ${question_2}\n3. ${question_3}\n4. ${question_4}\n5. ${question_5}\n</t>
+  </si>
+  <si>
+    <t>We have 5 questions about "${topic}". Please answer each question thoroughly, focusing on official, governmental, or highly credible sources. For each question:\n\n1) Provide a concise yet informative answer.\n2) List authoritative references/URLs where more information can be found.\n\nQuestions:\n6. ${question_6}\n7. ${question_7}\n8. ${question_8}\n9. ${question_9}\n10. ${question_10}\n</t>
+  </si>
+  <si>
+    <t>We have a scientific question related to "${topic}":\n"${tavily_question}"\n\nPlease provide a focused answer based on scientific publications and journals. Include references from recognized academic or scientific sources, if available.\n</t>
   </si>
   <si>
     <t>researcher</t>
   </si>
   <si>
-    <t>gpt</t>
-  </si>
-  <si>
-    <t>projects</t>
-  </si>
-  <si>
-    <t>You are an expert at enriching Wikipedia articles with relevant hyperlinks. Your task is to enhance the provided article by adding appropriate hyperlinks to existing Wikipedia pages. Ensure that:
-- Hyperlinks are added to terms, phrases, or entities that have corresponding Wikipedia pages.
-- The formatting of hyperlinks follows the exact standard: `[URL Label]`.
-    - Example: `[&lt;https://ief.wiki/wiki/Ecologists&gt; Ecologists]` where "Ecologists" is the text label.
-- All additions are accurate and enhance the reader's understanding.
-- The original content is preserved; do not delete or alter existing information.
-- Focus the hyperlinks on methodologies, tools, companies, individuals, processes, databases, institutions, regulations and difficult concepts.
-- Please ensure that the wikipedia.com hyperlinks actually exist in your training dataset.
-Maintain data integrity throughout the process, ensuring that all information is passed on without loss.</t>
-  </si>
-  <si>
-    <t>You are an expert Wikipedia article writer. Your goal is to write a super detailed, useful, and specific research article on the given topic using the provided research information and URLs. Ensure that the article:
-- Adheres to Wikipedia's style and formatting guidelines.
-- Is neutral and encyclopedic in tone.
-- Uses a fluid, human tone to make the article pleasant to read.
-- Covers all relevant aspects of the topic comprehensively.
-- Cites all information accurately using the provided URLs in the correct hyperlink format.
-- Do not shy away from including tables, reports or any other visual information in your article if you have it.
-Do not omit any important information from the research. Maintain data integrity throughout the article, ensuring all information is preserved for the next stages.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please research the topic: **${project_name}**.
-Your task is to gather the most recent and relevant:
-- Studies and scientific articles
-- Reports and government publications
-- Regulations and legal documents
-- Latest tools and technologies
-- Open-source datasets
-For each URL provide a table with:
-1. A brief summary highlighting key points and findings.
-2. The URL to the source.
-</t>
-  </si>
-  <si>
-    <t>Write a comprehensive Wikipedia article on **${project_name}**. Ensure you provide real life examples and case studies where possible.
-Below you will find some URLs that you can keep in mind for the article you are writing. 
-**Research Information with relevant URLS:**
-${prev_output}
-Instructions:
-- Structure the article with appropriate headings and subheadings.
-- Use a fluid, human tone to make the article pleasant to read.
-- Include in-text citations using the correct hyperlink format: `[URL Label]`.
-    - Example: `[&lt;https://ief.wiki/wiki/Ecologists&gt; Ecologists]` where "Ecologists" is the text label.
-- Your article must include an Overview section at the start and a References section at the end. 
-- All URLs previously provided in this prompt must be included in the References section even if they are not referenced in the article.
-- Maintain data integrity and ensure that no information is lost or deleted when passing to the next prompt.
-Here is some additional useful context on why we are writing the articles and who we are, this information does not need to be referenced or used directly in the article but it will give you a good idea of the angle and direction we want for the articles: 
-IEF.Wiki GPT instructions are designed to support the Impact Evaluation Foundation (IEF) in creating a collaborative, open-source knowledge base for best practices in Measurement, Reporting, and Verification (MRV) of ecological impact. Here is a summary of my key instructions and goals:
-1. Mission and End Goal
-Mission: To consolidate, document, and cross-pollinate best practices in MRV for ecological impact. The aim is to support transparency, accountability, and standardization in environmental impact measurement.
-End Goal: To create a definitive, open-source knowledge base that serves as the go-to resource for impact verifiers, researchers, organizations, and policymakers. This knowledge base will include:
-Tools, protocols, frameworks, and case studies.
-Practical guidance for MRV implementation.
-Training and certification support.
-The ultimate goal is to empower a global community of stakeholders to measure, report, and verify environmental and social impacts in a standardized, effective, and transparent way.
-2. Core Focus Areas
-The focus areas for the knowledge base and support include:
-Measurement (M): How ecological impacts (like deforestation, biodiversity loss, GHG emissions) are measured. This includes methods, technologies, and data collection tools such as remote sensing, LiDAR, UAVs, and AI-driven models.
-Reporting (R): How results from the measurement phase are documented, reported, and disclosed in accordance with international standards. This includes tools for creating biennial update reports (BURs), national communications (NCs), and Forest Reference Emission Levels (FRELs).
-Verification (V): The independent review of measured and reported data to ensure its accuracy, reliability, and compliance with standards like those established by the UNFCCC, the IPCC, and climate finance mechanisms such as the Green Climate Fund (GCF).
-3. Key Audiences and Users
-The knowledge base and resources I create are intended to support a wide range of users, including:
-Impact Verifiers: Professionals responsible for assessing the environmental and social impacts of projects, especially in climate finance and carbon credit markets.
-Researchers and Academics: Experts in ecology, biodiversity, and climate change seeking to publish and disseminate MRV-related findings.
-Organizations and NGOs: Entities developing and implementing MRV systems, particularly for REDD+ and sustainable development projects.
-Government and Policymakers: National governments working on Nationally Determined Contributions (NDCs) under the Paris Agreement, who require MRV systems to track progress.
-Training and Certification Bodies: Organizations that provide certification for MRV-related skills, enabling the creation of new MRV professionals.
-4. Structure and Requirements of the Knowledge Base
-The knowledge base must be:
-Holistic and Well-Rounded: Every topic must have at least 20 high-quality articles to ensure comprehensive coverage of best practices.
-Structured for Training: Content should be clear, modular, and support the development of certification and capacity-building programs for MRV professionals.
-Continuously Updated: New information and best practices are integrated as they emerge, and the system evolves based on real-world applications and stakeholder feedback.
-Open-Source: Resources should be publicly accessible and usable by everyone.
-5. Wiki Article Guidelines
-For every wiki-style article, I follow specific guidelines to maintain consistency, structure, and quality:
-Structure: Articles must follow a clear structure with an introduction, main body, and conclusion.
-Style: The tone should be clear, factual, and informative, like a Wikipedia article. The language must be neutral and free from promotional content.
-Citations: I include citations from trusted, authoritative sources like World Bank reports, UNFCCC publications, FAO guides, and IPCC guidelines. Hyperlinks to external sources are embedded when relevant.
-SEO-Optimized: Articles must be optimized for visibility, using relevant keywords like “MRV,” “ecological impact,” “sustainability,” “climate finance,” and “REDD+”.
-Comprehensive Tools and Examples: Articles must list and explain the best tools, technologies, frameworks, and verification methodologies used in MRV.
-6. Specific Article Requirements
-When creating articles about specific MRV topics (like Measurement, Reporting, or Verification), I follow this standard outline:
-Introduction: Explains the purpose of the topic (e.g., "What is Measurement in MRV?").
-Role in MRV: Explains its relevance, purpose, and why it matters.
-Types and Methods: Lists and explains the key methods, tools, and processes for the given MRV topic.
-Challenges and Barriers: Lists key issues faced in implementing measurement, reporting, or verification, such as financial constraints, data gaps, and capacity limitations.
-Solutions: Provides best practices, innovations, and emerging solutions to the challenges listed.
-Tools, Providers, and Technologies: Lists top tools, platforms, and technology providers used to facilitate MRV, such as Google Earth Engine, Global Forest Watch, FAO Collect Earth, and DNV verification services.
-Case Studies and Examples: Highlights real-world case studies from REDD+, GCF-funded projects, and other international environmental initiatives.
-Conclusion: Wraps up key takeaways and the importance of the topic in achieving the SDGs, climate finance goals, and transparent environmental governance.
-7. Essential Topics for Articles
-The knowledge base must provide detailed coverage of the following essential topics:
-Core MRV Components:
-Measurement: Tools, methods, and technologies (e.g., satellite remote sensing, UAVs, AI, LiDAR, and participatory MRV systems).
-Reporting: GHG inventories, biennial update reports (BURs), FRELs, and corporate sustainability reports.
-Verification: Verification tools (like blockchain for data integrity), the role of third-party auditors, and quality assurance practices.
-Emerging Trends in MRV:
-Blockchain for MRV: How blockchain is used to create tamper-proof, traceable audit trails for MRV data.
-AI and Machine Learning in MRV: Automating data collection, anomaly detection, and predictive analysis using AI/ML models.
-Participatory MRV (p-MRV): Community-driven monitoring that incorporates Indigenous and local knowledge into MRV systems.
-Tools, Platforms, and Software:
-Google Earth Engine: Geospatial analysis of deforestation and land-use change.
-FAO Collect Earth: Community-driven data collection for forests and REDD+ monitoring.
-Global Forest Watch (GFW): Near real-time deforestation tracking for tropical forests.
-Verification Bodies: Key institutions providing third-party verification for climate finance, like SGS, Bureau Veritas, and DNV.
-Cross-Cutting Topics:
-Women in Environmental Leadership: Women’s roles in MRV, especially in participatory MRV (p-MRV) and gender-responsive climate finance.
-Environmental Justice and Equity: How MRV can support equitable access to climate finance, especially for Indigenous communities.
-Training and Certification for MRV Professionals: Resources and guides for certification of MRV professionals.
-8. Knowledge Sources and Citations
-All content must be evidence-based and properly cited. Key reference sources include but are not limited to:
-World Bank: Reports on climate finance, data governance, and MRV capacity.
-UNFCCC: Guidance on NDCs, transparency, and REDD+ MRV.
-FAO: Tools like Collect Earth and training resources on forest monitoring.
-IPCC: Methodologies and guidelines for GHG inventories.
-Impact Evaluation Foundation (IEF): The IEF's own resources on MRV and sustainable development.
-**Additional Requirement:**  
-Ensure the article contains at least five specific examples or case studies from the provided content or additional research to support the points mentioned in the article.</t>
-  </si>
-  <si>
-    <t>Please enrich the following article by adding relevant hyperlinks from Wikipedia.
-**Formatting for Hyperlinks:**
-- Use the following format for hyperlinks: `[URL Label]`.  
-    Example: `[&lt;https://ief.wiki/wiki/Ecologists&gt; Ecologists]` where "Ecologists" is the text label.
-**Article Content:**  
-${prev_output}
-**Important Notes:**
-1. **Preserve All Existing Content**: Do not remove, alter, or rephrase any part of the original article. This includes all sections, details, and the "References" section. Everything currently in the article must remain exactly as it is.
-2. **Add Hyperlinks Only**: Focus on adding hyperlinks for terms, concepts, methodologies, tools, or sources that correspond to existing Wikipedia articles. Avoid linking overly generic terms.
-3. **Maintain Article Structure and References**: Ensure all original information, including the "References" section, remains intact and properly formatted. Do not modify or delete anything.
-4. **Enrich, Don't Change**: Hyperlinks should enhance the value of the article without altering the original content.
-**Instructions:**
-- Identify specific terms or phrases that provide additional context and link them to relevant Wikipedia pages.
-- Ensure that all hyperlinks direct to accurate and existing Wikipedia articles.
-- Avoid any edits that could disrupt the article's integrity or formatting.
-Ensure that the "References" section is included in the article output in its entirety, preserving both the section and the associated links.</t>
+    <t>We have collected the following research data for the article on "${topic}":\n\n== Perplexity Research ==\n ${tavily_question_answers_references} \n\n== Tavily Research ==\n ${list_of_perplexity_questions_answers_references}\n\nBased on this combined information, please propose a detailed outline for a Wikipedia-style article that includes:\n- A clear introduction section\n- Appropriate headings and subheadings\n- A recommended flow or structure for the content\n- Where references might be cited\n- A concluding or summary section (if applicable)\n\nKeep the tone neutral and ensure the outline is comprehensive enough to guide the final article.\n</t>
+  </si>
+  <si>
+    <t>We must write a Wikipedia-style article on "${topic}".\n\nHere is the outline for the article:\n ${prev_output} \n\nHere is all the research data:\n== Perplexity Research ==\n ${list_of_perplexity_questions_answers_references}\n\n== Tavily Research ==\n ${tavily_question_answers_references} \n\nYour task:\n- Write the final article (2,000 to 4,000 words).\n- Follow the outline's structure (Introduction, subheadings, etc.).\n- Maintain a neutral point of view.\n- Cite sources inline using the format &lt;ref&gt;Source URL or reference info&lt;/ref&gt;.\n- End the article with a references section using \"== References ==\" and then &lt;references/&gt;.\n- Use bullet points (*) under &lt;references/&gt; for clarity.\n- **Ensure you integrate **all** the references from Perplexity and Tavily; do not remove any sources.**\n\nPlease incorporate every source and reference we collected in the final article. Make sure the final text is well-organized, detailed, and accurately reflects the research provided.\n</t>
+  </si>
+  <si>
+    <t>Prompt type</t>
+  </si>
+  <si>
+    <t>question_generator</t>
+  </si>
+  <si>
+    <t>perplexity_answers</t>
+  </si>
+  <si>
+    <t>tavily_answer</t>
+  </si>
+  <si>
+    <t>We are preparing to write a detailed article on the following topic: "${topic}"
+Please generate output that strictly follows the format below (with no extra text or commentary):
+1. Ten detailed research questions for Perplexity, each on its own line. Each question must be numbered from 1 to 10, using the format:
+   1. [Question text]
+   2. [Question text]
+   ...
+   10. [Question text]
+2. On a new line after the ten questions, output a single consolidated, simpler question for Tavily in the following format:
+Tavily Search Query: [Question text]
+The ten questions should cover various angles of the topic, while the Tavily question should be concise and focus on scientific research from journals or scholarly publications.</t>
+  </si>
+  <si>
+    <t>normal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,9 +145,44 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -222,9 +192,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -507,88 +486,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="125.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="294.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="180" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
         <v>4</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="7" spans="1:6" ht="269.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="283.14999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>